<commit_message>
fixed bug for n-loci
</commit_message>
<xml_diff>
--- a/notes/parameter values.xlsx
+++ b/notes/parameter values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\Science\Manuscripts\trout-migration\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Kane\Documents\Manuscripts\Trout migration\trout-migration\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F576E8A-6AFA-4D78-8F7A-890C64DAA544}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD1E89F-2B1F-44BC-9BA0-D11A834B5123}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="3380" windowWidth="14400" windowHeight="7360" xr2:uid="{3D377FA1-CACB-4D4C-9953-864B3BCBAEC3}"/>
+    <workbookView xWindow="25980" yWindow="4470" windowWidth="11835" windowHeight="15435" xr2:uid="{3D377FA1-CACB-4D4C-9953-864B3BCBAEC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Parameter</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>0.26 - 1.9251</t>
+  </si>
+  <si>
+    <t>Mature natural mortality probability for resident morph under default conditions</t>
+  </si>
+  <si>
+    <t>Mature natural mortality probability for anadromous morph under default conditions</t>
+  </si>
+  <si>
+    <t>Thériault, V., Dunlop, E. S., Dieckmann, U., Bernatchez, L., &amp; Dodson, J. J. (2008). The impact of fishing‐induced mortality on the evolution of alternative life‐history tactics in brook charr. Evolutionary Applications, 1(2), 409-423.</t>
   </si>
 </sst>
 </file>
@@ -444,23 +453,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A4B5B4-4BD2-4933-B4E5-3BA7BF95B109}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -488,7 +497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -502,7 +511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -516,7 +525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -530,7 +539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -541,7 +550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -552,7 +561,30 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>0.88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minus time extension model
</commit_message>
<xml_diff>
--- a/notes/parameter values.xlsx
+++ b/notes/parameter values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Kane\Documents\Manuscripts\Trout migration\trout-migration\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\Science\Manuscripts\trout-migration\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD1E89F-2B1F-44BC-9BA0-D11A834B5123}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C458D3B-3A12-41FE-BFB5-BE75DAFFDBF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25980" yWindow="4470" windowWidth="11835" windowHeight="15435" xr2:uid="{3D377FA1-CACB-4D4C-9953-864B3BCBAEC3}"/>
+    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{3D377FA1-CACB-4D4C-9953-864B3BCBAEC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Parameter</t>
   </si>
@@ -42,15 +42,6 @@
     <t>Ref</t>
   </si>
   <si>
-    <t>Table 14.2</t>
-  </si>
-  <si>
-    <t>SEA TROUT: BIOLOGY, CONSERVATION AND MANAGEMENT</t>
-  </si>
-  <si>
-    <t>Harris and Milner 2004</t>
-  </si>
-  <si>
     <t>size at maturity (cm)</t>
   </si>
   <si>
@@ -84,22 +75,7 @@
     <t>Poole et al. 1996</t>
   </si>
   <si>
-    <t>Instantaneous total mortality rate (per year)</t>
-  </si>
-  <si>
-    <t>Arslan et al. 2007</t>
-  </si>
-  <si>
-    <t>0.26 - 1.9251</t>
-  </si>
-  <si>
-    <t>Mature natural mortality probability for resident morph under default conditions</t>
-  </si>
-  <si>
-    <t>Mature natural mortality probability for anadromous morph under default conditions</t>
-  </si>
-  <si>
-    <t>Thériault, V., Dunlop, E. S., Dieckmann, U., Bernatchez, L., &amp; Dodson, J. J. (2008). The impact of fishing‐induced mortality on the evolution of alternative life‐history tactics in brook charr. Evolutionary Applications, 1(2), 409-423.</t>
+    <t>Table 14.2; Harris, G., &amp; Milner, N. (Eds.). (2008). Sea trout: biology, conservation and management. John Wiley &amp; Sons.</t>
   </si>
 </sst>
 </file>
@@ -453,23 +429,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A4B5B4-4BD2-4933-B4E5-3BA7BF95B109}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,108 +455,60 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
-        <v>0.88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>